<commit_message>
Added support for GHP Log types and the app now logs the console
</commit_message>
<xml_diff>
--- a/dist/production_pc.xlsx
+++ b/dist/production_pc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vt1.vitesco.com\SMT\didt1083\01_MES_PUBLIC\1.6.Production Errors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vt1.vitesco.com\SMT\didt1083\02_MES_TEAM\2.4. Applications\UnitIDsearch 1.7 -do not use-\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D25792-49F5-4D15-A3BC-C0229D49CA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13590"/>
   </bookViews>
   <sheets>
     <sheet name="production_pc" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="300">
   <si>
     <t>Alfa Giorgio &amp; GM Subassy</t>
   </si>
@@ -908,13 +907,25 @@
   </si>
   <si>
     <t>P1400 Pump F</t>
+  </si>
+  <si>
+    <t>\\10.214.86.219\d$\MES_Robust\GHP_19 4.0.12\P85SCR_L04S01\GHPService_P85SCR</t>
+  </si>
+  <si>
+    <t>SCR 4 - P85 Service</t>
+  </si>
+  <si>
+    <t>SCR 3 - P85 Service</t>
+  </si>
+  <si>
+    <t>\\10.214.85.219\d$\MES_GHP Robust\GHP_18 4.0.3.0\P85SCR_L03S01\GHPService_P85SCR_L03S01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1767,20 +1778,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150:XFD150"/>
+      <selection activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>294</v>
       </c>
@@ -1788,7 +1799,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1796,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1804,7 +1815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1820,7 +1831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1828,7 +1839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -1836,7 +1847,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>187</v>
       </c>
@@ -1844,7 +1855,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1852,7 +1863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1860,7 +1871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1868,7 +1879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1876,7 +1887,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1884,7 +1895,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1892,7 +1903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1900,7 +1911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1908,7 +1919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1916,7 +1927,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1924,7 +1935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1932,7 +1943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1940,7 +1951,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1948,7 +1959,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1956,7 +1967,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1964,7 +1975,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -1972,7 +1983,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -1980,7 +1991,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>207</v>
       </c>
@@ -1988,7 +1999,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>209</v>
       </c>
@@ -1996,7 +2007,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>211</v>
       </c>
@@ -2004,7 +2015,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>213</v>
       </c>
@@ -2012,7 +2023,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>295</v>
       </c>
@@ -2020,7 +2031,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -2028,7 +2039,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>217</v>
       </c>
@@ -2036,7 +2047,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>219</v>
       </c>
@@ -2044,7 +2055,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>221</v>
       </c>
@@ -2052,7 +2063,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -2060,7 +2071,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>225</v>
       </c>
@@ -2068,7 +2079,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>227</v>
       </c>
@@ -2076,7 +2087,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>229</v>
       </c>
@@ -2084,7 +2095,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>231</v>
       </c>
@@ -2092,7 +2103,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>233</v>
       </c>
@@ -2100,7 +2111,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>234</v>
       </c>
@@ -2108,7 +2119,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>236</v>
       </c>
@@ -2116,7 +2127,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>238</v>
       </c>
@@ -2124,7 +2135,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>240</v>
       </c>
@@ -2132,7 +2143,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>242</v>
       </c>
@@ -2140,7 +2151,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>244</v>
       </c>
@@ -2148,7 +2159,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>246</v>
       </c>
@@ -2156,7 +2167,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>189</v>
       </c>
@@ -2164,7 +2175,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -2172,7 +2183,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>191</v>
       </c>
@@ -2180,7 +2191,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>192</v>
       </c>
@@ -2188,7 +2199,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>193</v>
       </c>
@@ -2196,7 +2207,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>194</v>
       </c>
@@ -2204,7 +2215,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>196</v>
       </c>
@@ -2212,7 +2223,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>254</v>
       </c>
@@ -2220,7 +2231,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>256</v>
       </c>
@@ -2228,7 +2239,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>258</v>
       </c>
@@ -2236,7 +2247,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>260</v>
       </c>
@@ -2244,7 +2255,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>262</v>
       </c>
@@ -2252,7 +2263,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>264</v>
       </c>
@@ -2260,7 +2271,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>266</v>
       </c>
@@ -2268,7 +2279,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>268</v>
       </c>
@@ -2276,7 +2287,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>270</v>
       </c>
@@ -2284,7 +2295,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -2292,7 +2303,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -2300,7 +2311,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -2308,7 +2319,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -2316,7 +2327,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -2324,7 +2335,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>53</v>
       </c>
@@ -2340,7 +2351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -2348,7 +2359,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>57</v>
       </c>
@@ -2356,7 +2367,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>59</v>
       </c>
@@ -2364,7 +2375,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>61</v>
       </c>
@@ -2372,7 +2383,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -2380,7 +2391,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -2388,7 +2399,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -2396,12 +2407,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>69</v>
       </c>
@@ -2409,7 +2420,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>71</v>
       </c>
@@ -2417,7 +2428,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>73</v>
       </c>
@@ -2425,7 +2436,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>75</v>
       </c>
@@ -2433,7 +2444,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -2441,7 +2452,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>197</v>
       </c>
@@ -2449,7 +2460,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -2457,7 +2468,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>81</v>
       </c>
@@ -2465,7 +2476,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>83</v>
       </c>
@@ -2473,7 +2484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -2481,7 +2492,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -2489,7 +2500,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2497,7 +2508,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -2505,7 +2516,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -2513,7 +2524,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -2521,7 +2532,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>273</v>
       </c>
@@ -2529,7 +2540,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>275</v>
       </c>
@@ -2537,7 +2548,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>277</v>
       </c>
@@ -2545,7 +2556,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>279</v>
       </c>
@@ -2553,7 +2564,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>281</v>
       </c>
@@ -2561,7 +2572,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>283</v>
       </c>
@@ -2569,7 +2580,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>285</v>
       </c>
@@ -2577,7 +2588,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>287</v>
       </c>
@@ -2585,7 +2596,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>289</v>
       </c>
@@ -2593,7 +2604,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>291</v>
       </c>
@@ -2601,7 +2612,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="14.25" customHeight="1">
       <c r="A104" t="s">
         <v>97</v>
       </c>
@@ -2609,7 +2620,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
         <v>99</v>
       </c>
@@ -2617,7 +2628,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -2625,7 +2636,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>103</v>
       </c>
@@ -2633,7 +2644,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
         <v>105</v>
       </c>
@@ -2641,7 +2652,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2649,7 +2660,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2657,7 +2668,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -2665,7 +2676,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -2673,7 +2684,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>115</v>
       </c>
@@ -2681,7 +2692,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>117</v>
       </c>
@@ -2689,7 +2700,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -2697,7 +2708,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>121</v>
       </c>
@@ -2705,7 +2716,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -2713,7 +2724,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -2721,7 +2732,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
         <v>127</v>
       </c>
@@ -2729,7 +2740,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
         <v>129</v>
       </c>
@@ -2737,7 +2748,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
         <v>131</v>
       </c>
@@ -2745,7 +2756,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
         <v>133</v>
       </c>
@@ -2753,7 +2764,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
         <v>135</v>
       </c>
@@ -2761,7 +2772,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
         <v>137</v>
       </c>
@@ -2769,7 +2780,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -2777,7 +2788,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -2785,7 +2796,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
         <v>143</v>
       </c>
@@ -2793,7 +2804,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
         <v>145</v>
       </c>
@@ -2801,7 +2812,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2">
       <c r="A129" t="s">
         <v>147</v>
       </c>
@@ -2809,7 +2820,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
         <v>149</v>
       </c>
@@ -2817,7 +2828,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>151</v>
       </c>
@@ -2825,7 +2836,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>153</v>
       </c>
@@ -2833,7 +2844,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>155</v>
       </c>
@@ -2841,131 +2852,147 @@
         <v>156</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
+        <v>298</v>
+      </c>
+      <c r="B134" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
         <v>157</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>297</v>
+      </c>
+      <c r="B136" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
         <v>159</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B137" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
         <v>161</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B138" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
         <v>163</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B139" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
         <v>165</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B140" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
         <v>167</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B141" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
         <v>169</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B142" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
         <v>199</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B143" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
         <v>201</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B144" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
         <v>171</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B145" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
         <v>173</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B146" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
         <v>175</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B147" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
         <v>177</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B148" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
         <v>179</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B149" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
         <v>181</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B150" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
         <v>183</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B151" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bug where SN pairs are doubled, redefined buttons and checkbox names. Final Version
</commit_message>
<xml_diff>
--- a/dist/production_pc.xlsx
+++ b/dist/production_pc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vt1.vitesco.com\SMT\didt1083\02_MES_TEAM\2.4. Applications\UnitIDsearch 1.7 -do not use-\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vitesco-my.sharepoint.com/personal/uiv55706_vitesco_com/Documents/DEV/UnitIDsearch/dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_5283C9689B861E95D4A975DCEC343AC9AD06B540" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26FA03C2-10BE-46BD-A2C7-697FF341414F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13590"/>
+    <workbookView xWindow="14385" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_pc" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="297">
   <si>
     <t>Alfa Giorgio &amp; GM Subassy</t>
   </si>
@@ -837,9 +838,6 @@
     <t>\\10.222.173.66\c$</t>
   </si>
   <si>
-    <t>MES2MES Server</t>
-  </si>
-  <si>
     <t>PEU Main Line</t>
   </si>
   <si>
@@ -909,23 +907,17 @@
     <t>P1400 Pump F</t>
   </si>
   <si>
-    <t>\\10.214.86.219\d$\MES_Robust\GHP_19 4.0.12\P85SCR_L04S01\GHPService_P85SCR</t>
-  </si>
-  <si>
-    <t>SCR 4 - P85 Service</t>
-  </si>
-  <si>
-    <t>SCR 3 - P85 Service</t>
-  </si>
-  <si>
-    <t>\\10.214.85.219\d$\MES_GHP Robust\GHP_18 4.0.3.0\P85SCR_L03S01\GHPService_P85SCR_L03S01</t>
+    <t>Test SCR_local_P70</t>
+  </si>
+  <si>
+    <t>C:\Users\uiv55706\OneDrive - Vitesco Technologies\MES\MES_Clients\1.2.2. SCR_VA\Rework</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1778,28 +1770,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B151"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="H145" sqref="H145"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.75" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1807,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1815,7 +1807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1823,7 +1815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1831,7 +1823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1839,7 +1831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>185</v>
       </c>
@@ -1847,7 +1839,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>187</v>
       </c>
@@ -1855,7 +1847,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1863,7 +1855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1871,7 +1863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1879,7 +1871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1887,7 +1879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1895,7 +1887,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1903,7 +1895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1911,7 +1903,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1919,7 +1911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1927,7 +1919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1935,7 +1927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1943,7 +1935,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1951,7 +1943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1959,7 +1951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1967,7 +1959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1975,7 +1967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -1983,7 +1975,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -1991,7 +1983,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>207</v>
       </c>
@@ -1999,7 +1991,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>209</v>
       </c>
@@ -2007,7 +1999,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>211</v>
       </c>
@@ -2015,7 +2007,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>213</v>
       </c>
@@ -2023,15 +2015,15 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -2039,7 +2031,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>217</v>
       </c>
@@ -2047,7 +2039,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>219</v>
       </c>
@@ -2055,7 +2047,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>221</v>
       </c>
@@ -2063,7 +2055,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -2071,7 +2063,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>225</v>
       </c>
@@ -2079,7 +2071,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>227</v>
       </c>
@@ -2087,7 +2079,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>229</v>
       </c>
@@ -2095,7 +2087,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>231</v>
       </c>
@@ -2103,7 +2095,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>233</v>
       </c>
@@ -2111,7 +2103,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>234</v>
       </c>
@@ -2119,7 +2111,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>236</v>
       </c>
@@ -2127,7 +2119,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>238</v>
       </c>
@@ -2135,7 +2127,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>240</v>
       </c>
@@ -2143,7 +2135,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>242</v>
       </c>
@@ -2151,7 +2143,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>244</v>
       </c>
@@ -2159,7 +2151,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>246</v>
       </c>
@@ -2167,7 +2159,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>189</v>
       </c>
@@ -2175,7 +2167,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -2183,7 +2175,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>191</v>
       </c>
@@ -2191,7 +2183,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>192</v>
       </c>
@@ -2199,7 +2191,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>193</v>
       </c>
@@ -2207,7 +2199,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>194</v>
       </c>
@@ -2215,7 +2207,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>196</v>
       </c>
@@ -2223,7 +2215,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>254</v>
       </c>
@@ -2231,7 +2223,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>256</v>
       </c>
@@ -2239,7 +2231,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>258</v>
       </c>
@@ -2247,7 +2239,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>260</v>
       </c>
@@ -2255,7 +2247,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>262</v>
       </c>
@@ -2263,7 +2255,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>264</v>
       </c>
@@ -2271,7 +2263,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>266</v>
       </c>
@@ -2279,7 +2271,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>268</v>
       </c>
@@ -2287,7 +2279,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>270</v>
       </c>
@@ -2295,7 +2287,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -2303,7 +2295,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>43</v>
       </c>
@@ -2311,7 +2303,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>45</v>
       </c>
@@ -2319,7 +2311,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -2327,7 +2319,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -2335,7 +2327,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -2343,7 +2335,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>53</v>
       </c>
@@ -2351,7 +2343,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -2359,7 +2351,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>57</v>
       </c>
@@ -2367,7 +2359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>59</v>
       </c>
@@ -2375,7 +2367,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>61</v>
       </c>
@@ -2383,7 +2375,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -2391,7 +2383,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>65</v>
       </c>
@@ -2399,7 +2391,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -2407,593 +2399,580 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>75</v>
+      </c>
+      <c r="B81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>197</v>
+      </c>
+      <c r="B83" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
-        <v>69</v>
-      </c>
-      <c r="B79" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
-        <v>71</v>
-      </c>
-      <c r="B80" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
-        <v>73</v>
-      </c>
-      <c r="B81" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
-        <v>75</v>
-      </c>
-      <c r="B82" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
-        <v>77</v>
-      </c>
-      <c r="B83" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>197</v>
-      </c>
-      <c r="B84" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>79</v>
-      </c>
-      <c r="B85" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>81</v>
-      </c>
-      <c r="B86" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
-        <v>83</v>
-      </c>
-      <c r="B87" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>93</v>
-      </c>
-      <c r="B92" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>95</v>
-      </c>
       <c r="B93" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B94" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B95" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B96" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B97" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B98" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B99" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B100" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B101" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B102" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>291</v>
+        <v>97</v>
       </c>
       <c r="B103" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="14.25" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B112" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B113" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B115" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B116" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B117" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B118" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B120" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B122" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B123" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B124" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B125" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B126" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B127" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B128" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B129" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B130" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B131" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B132" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B133" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>298</v>
+        <v>159</v>
       </c>
       <c r="B134" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B135" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>297</v>
+        <v>163</v>
       </c>
       <c r="B136" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>165</v>
+      </c>
+      <c r="B137" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>167</v>
+      </c>
+      <c r="B138" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>169</v>
+      </c>
+      <c r="B139" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>199</v>
+      </c>
+      <c r="B140" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>201</v>
+      </c>
+      <c r="B141" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>171</v>
+      </c>
+      <c r="B142" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>173</v>
+      </c>
+      <c r="B143" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>175</v>
+      </c>
+      <c r="B144" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>177</v>
+      </c>
+      <c r="B145" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>179</v>
+      </c>
+      <c r="B146" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>181</v>
+      </c>
+      <c r="B147" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>183</v>
+      </c>
+      <c r="B148" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>295</v>
+      </c>
+      <c r="B149" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
-      <c r="A137" t="s">
-        <v>159</v>
-      </c>
-      <c r="B137" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
-      <c r="A138" t="s">
-        <v>161</v>
-      </c>
-      <c r="B138" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" t="s">
-        <v>163</v>
-      </c>
-      <c r="B139" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" t="s">
-        <v>165</v>
-      </c>
-      <c r="B140" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" t="s">
-        <v>167</v>
-      </c>
-      <c r="B141" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
-      <c r="A142" t="s">
-        <v>169</v>
-      </c>
-      <c r="B142" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" t="s">
-        <v>199</v>
-      </c>
-      <c r="B143" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
-      <c r="A144" t="s">
-        <v>201</v>
-      </c>
-      <c r="B144" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" t="s">
-        <v>171</v>
-      </c>
-      <c r="B145" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
-      <c r="A146" t="s">
-        <v>173</v>
-      </c>
-      <c r="B146" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
-      <c r="A147" t="s">
-        <v>175</v>
-      </c>
-      <c r="B147" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
-      <c r="A148" t="s">
-        <v>177</v>
-      </c>
-      <c r="B148" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
-      <c r="A149" t="s">
-        <v>179</v>
-      </c>
-      <c r="B149" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
-      <c r="A150" t="s">
-        <v>181</v>
-      </c>
-      <c r="B150" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
-      <c r="A151" t="s">
-        <v>183</v>
-      </c>
-      <c r="B151" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>